<commit_message>
app: able update rate, tasks list by yearly ...
</commit_message>
<xml_diff>
--- a/docs/timsheet.xlsx
+++ b/docs/timsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19AE8FA-A70C-4536-90C5-2D9CA0F9711F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69893360-7F3F-4BBD-8DAE-0975D977887B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Start</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>12/23/2019</t>
+  </si>
+  <si>
+    <t>12/27/2019</t>
+  </si>
+  <si>
+    <t>12/26/2019</t>
+  </si>
+  <si>
+    <t>12/25/2019</t>
+  </si>
+  <si>
+    <t>12/24/2019</t>
+  </si>
+  <si>
+    <t>12/28/2019</t>
+  </si>
+  <si>
+    <t>12/29/2019</t>
+  </si>
+  <si>
+    <t>PPD</t>
   </si>
 </sst>
 </file>
@@ -136,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -146,6 +167,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -426,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,8 +459,9 @@
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
     <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -552,7 +575,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" ref="D8:D21" si="0">C8-B8</f>
+        <f t="shared" ref="D8:D25" si="0">C8-B8</f>
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
@@ -651,7 +674,7 @@
       </c>
       <c r="G14" s="7">
         <f>SUM(D2:D38)</f>
-        <v>2.7680439814814815</v>
+        <v>4.7402662037037038</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -684,7 +707,7 @@
         <v>0.10416666666666674</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -699,7 +722,7 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -714,7 +737,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -729,7 +752,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -744,10 +767,90 @@
         <v>0.20833333333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>0.51388888888888884</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.52083333333333326</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.4861111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
presentation update & timesheet
</commit_message>
<xml_diff>
--- a/docs/timsheet.xlsx
+++ b/docs/timsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBC90D0-A17C-42A5-ABD3-91C75C62687E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DED72ED-28CE-4D35-9C9A-F93C5284C3D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
       </c>
       <c r="G14" s="9">
         <f>SUM(D2:D38)</f>
-        <v>7.04582175925926</v>
+        <v>7.60832175925926</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
       </c>
       <c r="G15" s="12">
         <f>G14*5</f>
-        <v>35.229108796296302</v>
+        <v>38.041608796296302</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -960,6 +960,36 @@
       <c r="D31" s="4">
         <f t="shared" si="0"/>
         <v>0.375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>43922</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" ref="D32" si="1">C32-B32</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>43952</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" ref="D33" si="2">C33-B33</f>
+        <v>0.4375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>